<commit_message>
Arreglado procesos de creación de puestos y asignación de empleados al distributivo
</commit_message>
<xml_diff>
--- a/WebAppTH/bd.webappth.web/wwwroot/DocumentoCapacitacion/Reportados/1.xlsx
+++ b/WebAppTH/bd.webappth.web/wwwroot/DocumentoCapacitacion/Reportados/1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriano\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carolina Peña\Dropbox\CAROLINAPENA\MANUALES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{52EE13A0-4E26-4A50-8281-5796594C3C24}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A53B9DDC-1B93-4BE9-B491-149CCDF4ACAC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{6B2C13AD-1B7B-4C89-B9B9-FC5F211352C1}"/>
   </bookViews>
@@ -526,7 +526,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,6 +540,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -562,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -575,6 +581,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -891,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1CD2495-498D-4338-BCBD-B97147290489}">
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:U1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,8 +977,8 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="108" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>213453232</v>
+      <c r="A2" s="6">
+        <v>22323232</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>21</v>
@@ -1038,8 +1045,8 @@
       </c>
     </row>
     <row r="3" spans="1:22" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>213453232</v>
+      <c r="A3" s="6">
+        <v>22323232</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
@@ -1106,8 +1113,8 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="132" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>213453232</v>
+      <c r="A4" s="6">
+        <v>22323232</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>21</v>
@@ -1171,8 +1178,8 @@
       </c>
     </row>
     <row r="5" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>213453232</v>
+      <c r="A5" s="6">
+        <v>22323232</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
@@ -1236,8 +1243,8 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>213453232</v>
+      <c r="A6" s="6">
+        <v>22323232</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>21</v>
@@ -1301,8 +1308,8 @@
       </c>
     </row>
     <row r="7" spans="1:22" ht="48" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>213453232</v>
+      <c r="A7" s="6">
+        <v>22323232</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
@@ -1366,8 +1373,8 @@
       </c>
     </row>
     <row r="8" spans="1:22" ht="48" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>213453232</v>
+      <c r="A8" s="6">
+        <v>22323232</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -1431,8 +1438,8 @@
       </c>
     </row>
     <row r="9" spans="1:22" ht="108" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>213453232</v>
+      <c r="A9" s="6">
+        <v>22323232</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
@@ -1496,8 +1503,8 @@
       </c>
     </row>
     <row r="10" spans="1:22" ht="132" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>213453232</v>
+      <c r="A10" s="6">
+        <v>22323232</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -1561,8 +1568,8 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="144" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>213453232</v>
+      <c r="A11" s="6">
+        <v>22323232</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
@@ -1626,8 +1633,8 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="108" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>213453232</v>
+      <c r="A12" s="6">
+        <v>22323232</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>21</v>
@@ -1691,8 +1698,8 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="96" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>213453232</v>
+      <c r="A13" s="6">
+        <v>22323232</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>21</v>
@@ -1756,8 +1763,8 @@
       </c>
     </row>
     <row r="14" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>213453232</v>
+      <c r="A14" s="6">
+        <v>22323232</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>21</v>
@@ -1821,8 +1828,8 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="96" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>213453232</v>
+      <c r="A15" s="6">
+        <v>22323232</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>21</v>
@@ -1886,8 +1893,8 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="84" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>213453232</v>
+      <c r="A16" s="6">
+        <v>22323232</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>21</v>
@@ -1951,8 +1958,8 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>213453232</v>
+      <c r="A17" s="6">
+        <v>22323232</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
@@ -2016,8 +2023,8 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="132" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>213453232</v>
+      <c r="A18" s="6">
+        <v>22323232</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>21</v>
@@ -2081,8 +2088,8 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>213453232</v>
+      <c r="A19" s="6">
+        <v>22323232</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>21</v>
@@ -2146,8 +2153,8 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>213453232</v>
+      <c r="A20" s="6">
+        <v>22323232</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>21</v>
@@ -2211,8 +2218,8 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>213453232</v>
+      <c r="A21" s="6">
+        <v>22323232</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
@@ -2276,8 +2283,8 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>213453232</v>
+      <c r="A22" s="6">
+        <v>22323232</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
@@ -2341,8 +2348,8 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>213453232</v>
+      <c r="A23" s="6">
+        <v>22323232</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>21</v>
@@ -2406,8 +2413,8 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="72" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>213453232</v>
+      <c r="A24" s="6">
+        <v>22323232</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
@@ -2471,8 +2478,8 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="96" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>213453232</v>
+      <c r="A25" s="6">
+        <v>22323232</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -2536,8 +2543,8 @@
       </c>
     </row>
     <row r="26" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>213453232</v>
+      <c r="A26" s="6">
+        <v>22323232</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>21</v>
@@ -2601,8 +2608,8 @@
       </c>
     </row>
     <row r="27" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>213453232</v>
+      <c r="A27" s="6">
+        <v>22323232</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>21</v>
@@ -2666,8 +2673,8 @@
       </c>
     </row>
     <row r="28" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>213453232</v>
+      <c r="A28" s="6">
+        <v>22323232</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>21</v>
@@ -2731,8 +2738,8 @@
       </c>
     </row>
     <row r="29" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>213453232</v>
+      <c r="A29" s="6">
+        <v>22323232</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>21</v>
@@ -2796,8 +2803,8 @@
       </c>
     </row>
     <row r="30" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>213453232</v>
+      <c r="A30" s="6">
+        <v>22323232</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>21</v>
@@ -2861,8 +2868,8 @@
       </c>
     </row>
     <row r="31" spans="1:21" ht="72" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>213453232</v>
+      <c r="A31" s="6">
+        <v>22323232</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>21</v>
@@ -2926,8 +2933,8 @@
       </c>
     </row>
     <row r="32" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>213453232</v>
+      <c r="A32" s="6">
+        <v>22323232</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>21</v>
@@ -2991,8 +2998,8 @@
       </c>
     </row>
     <row r="33" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>213453232</v>
+      <c r="A33" s="6">
+        <v>22323232</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>21</v>
@@ -3056,8 +3063,8 @@
       </c>
     </row>
     <row r="34" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>213453232</v>
+      <c r="A34" s="6">
+        <v>22323232</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>21</v>
@@ -3121,8 +3128,8 @@
       </c>
     </row>
     <row r="35" spans="1:21" ht="84" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>213453232</v>
+      <c r="A35" s="6">
+        <v>22323232</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>21</v>

</xml_diff>